<commit_message>
edit tf_nn file to grab values from spreadsheet and display them
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -2177,29 +2177,29 @@
   </sheetPr>
   <dimension ref="1:851"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H89" activeCellId="0" sqref="H89"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="5" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="5" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="5" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="33.75"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="5" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="5" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="5" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="5" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="5" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="111.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9807,7 +9807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="17" t="n">
         <v>42810</v>
       </c>
@@ -9843,8 +9843,9 @@
       <c r="M184" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="185" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N184" s="0"/>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="17" t="n">
         <v>42829</v>
       </c>
@@ -9880,8 +9881,9 @@
       <c r="M185" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="186" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N185" s="0"/>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="17" t="n">
         <v>42843</v>
       </c>
@@ -9917,8 +9919,9 @@
       <c r="M186" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="187" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N186" s="0"/>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="17" t="n">
         <v>42831</v>
       </c>
@@ -9952,8 +9955,9 @@
       <c r="M187" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="188" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N187" s="0"/>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="17" t="n">
         <v>42935</v>
       </c>
@@ -9987,8 +9991,9 @@
       <c r="M188" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="189" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N188" s="0"/>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="17" t="n">
         <v>42844</v>
       </c>
@@ -10024,8 +10029,9 @@
       <c r="M189" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="190" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N189" s="0"/>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="17" t="n">
         <v>42935</v>
       </c>
@@ -10059,8 +10065,9 @@
       <c r="M190" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="191" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N190" s="0"/>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="30" t="n">
         <v>42999</v>
       </c>
@@ -10094,8 +10101,9 @@
       <c r="M191" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="192" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N191" s="0"/>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="17" t="n">
         <v>42662</v>
       </c>
@@ -10129,8 +10137,9 @@
       <c r="M192" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="193" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N192" s="0"/>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="17" t="n">
         <v>42676</v>
       </c>
@@ -10164,8 +10173,9 @@
       <c r="M193" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="194" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N193" s="0"/>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="17" t="n">
         <v>42872</v>
       </c>
@@ -10199,8 +10209,9 @@
       <c r="M194" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="195" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N194" s="0"/>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="17" t="n">
         <v>42677</v>
       </c>
@@ -10234,8 +10245,9 @@
       <c r="M195" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="196" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N195" s="0"/>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="17" t="n">
         <v>42808</v>
       </c>
@@ -10269,8 +10281,9 @@
       <c r="M196" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="197" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N196" s="0"/>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="17" t="n">
         <v>42837</v>
       </c>
@@ -10306,8 +10319,9 @@
       <c r="M197" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="198" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N197" s="0"/>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="17" t="n">
         <v>42872</v>
       </c>
@@ -10341,8 +10355,9 @@
       <c r="M198" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="199" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N198" s="0"/>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="17" t="n">
         <v>42900</v>
       </c>
@@ -10376,8 +10391,9 @@
       <c r="M199" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="200" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N199" s="0"/>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="17" t="n">
         <v>42928</v>
       </c>
@@ -10411,8 +10427,9 @@
       <c r="M200" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="201" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N200" s="0"/>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="17" t="n">
         <v>42963</v>
       </c>
@@ -10446,8 +10463,9 @@
       <c r="M201" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="202" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N201" s="0"/>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="17" t="n">
         <v>42822</v>
       </c>
@@ -10481,8 +10499,9 @@
       <c r="M202" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="203" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N202" s="0"/>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="17" t="n">
         <v>42837</v>
       </c>
@@ -10516,8 +10535,9 @@
       <c r="M203" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="204" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N203" s="0"/>
+    </row>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="17" t="n">
         <v>42873</v>
       </c>
@@ -10551,8 +10571,9 @@
       <c r="M204" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="205" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N204" s="0"/>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="17" t="n">
         <v>42951</v>
       </c>
@@ -10586,8 +10607,9 @@
       <c r="M205" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="206" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N205" s="0"/>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="17" t="n">
         <v>42822</v>
       </c>
@@ -10621,8 +10643,9 @@
       <c r="M206" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="207" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N206" s="0"/>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="17" t="n">
         <v>42937</v>
       </c>
@@ -10656,8 +10679,9 @@
       <c r="M207" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="208" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N207" s="0"/>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="17" t="n">
         <v>42905</v>
       </c>
@@ -10693,8 +10717,9 @@
       <c r="M208" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="209" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N208" s="0"/>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="17" t="n">
         <v>42835</v>
       </c>
@@ -10730,8 +10755,9 @@
       <c r="M209" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="210" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N209" s="0"/>
+    </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="17" t="n">
         <v>42935</v>
       </c>
@@ -10765,8 +10791,9 @@
       <c r="M210" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="211" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N210" s="0"/>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="17" t="n">
         <v>42643</v>
       </c>
@@ -10802,8 +10829,9 @@
       <c r="M211" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="212" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N211" s="0"/>
+    </row>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="17" t="n">
         <v>42776</v>
       </c>
@@ -10837,8 +10865,9 @@
       <c r="M212" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="213" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N212" s="0"/>
+    </row>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="17" t="n">
         <v>42905</v>
       </c>
@@ -10876,8 +10905,9 @@
       <c r="M213" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="214" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N213" s="0"/>
+    </row>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="17" t="n">
         <v>42951</v>
       </c>
@@ -10915,8 +10945,9 @@
       <c r="M214" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="215" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N214" s="0"/>
+    </row>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="30" t="n">
         <v>43018</v>
       </c>
@@ -10950,8 +10981,9 @@
       <c r="M215" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="216" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N215" s="0"/>
+    </row>
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="17" t="n">
         <v>42905</v>
       </c>
@@ -10987,8 +11019,9 @@
       <c r="M216" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="217" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N216" s="0"/>
+    </row>
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="17" t="n">
         <v>42962</v>
       </c>
@@ -11024,8 +11057,9 @@
       <c r="M217" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="218" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N217" s="0"/>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="17" t="n">
         <v>42873</v>
       </c>
@@ -11061,8 +11095,9 @@
       <c r="M218" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="219" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N218" s="0"/>
+    </row>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="17" t="n">
         <v>42958</v>
       </c>
@@ -11098,8 +11133,9 @@
       <c r="M219" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="220" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N219" s="0"/>
+    </row>
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="30" t="n">
         <v>42991</v>
       </c>
@@ -11135,8 +11171,9 @@
       <c r="M220" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="221" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N220" s="0"/>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="30" t="n">
         <v>43019</v>
       </c>
@@ -11172,8 +11209,9 @@
       <c r="M221" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="222" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N221" s="0"/>
+    </row>
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="30" t="n">
         <v>43054</v>
       </c>
@@ -11209,8 +11247,9 @@
       <c r="M222" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="223" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N222" s="0"/>
+    </row>
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="30" t="n">
         <v>43082</v>
       </c>
@@ -11246,8 +11285,9 @@
       <c r="M223" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="224" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N223" s="0"/>
+    </row>
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="17" t="n">
         <v>42874</v>
       </c>
@@ -11283,8 +11323,9 @@
       <c r="M224" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="225" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N224" s="0"/>
+    </row>
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="17" t="n">
         <v>42951</v>
       </c>
@@ -11320,8 +11361,9 @@
       <c r="M225" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="226" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N225" s="0"/>
+    </row>
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="30" t="n">
         <v>42984</v>
       </c>
@@ -11357,8 +11399,9 @@
       <c r="M226" s="34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="227" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N226" s="0"/>
+    </row>
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="30" t="n">
         <v>43019</v>
       </c>
@@ -11396,8 +11439,9 @@
       <c r="M227" s="34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="228" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N227" s="0"/>
+    </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="30" t="n">
         <v>43054</v>
       </c>
@@ -11433,8 +11477,9 @@
       <c r="M228" s="34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="229" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N228" s="0"/>
+    </row>
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="30" t="n">
         <v>43082</v>
       </c>
@@ -11470,6 +11515,7 @@
       <c r="M229" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N229" s="0"/>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="17" t="n">
@@ -13489,6 +13535,7 @@
       <c r="M283" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N283" s="0"/>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="17" t="n">
@@ -13526,6 +13573,7 @@
       <c r="M284" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N284" s="0"/>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="17"/>
@@ -13551,6 +13599,7 @@
       <c r="K285" s="21"/>
       <c r="L285" s="21"/>
       <c r="M285" s="22"/>
+      <c r="N285" s="0"/>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="17" t="n">
@@ -13586,6 +13635,7 @@
       <c r="M286" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N286" s="0"/>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="17" t="n">
@@ -13621,6 +13671,7 @@
       <c r="M287" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N287" s="0"/>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="30" t="n">
@@ -13656,6 +13707,7 @@
       <c r="M288" s="34" t="s">
         <v>19</v>
       </c>
+      <c r="N288" s="0"/>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="17" t="n">
@@ -13693,6 +13745,7 @@
       <c r="M289" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N289" s="0"/>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="17" t="n">
@@ -13730,6 +13783,7 @@
       <c r="M290" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N290" s="0"/>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="17" t="n">
@@ -13767,6 +13821,7 @@
       <c r="M291" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N291" s="0"/>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="30" t="n">
@@ -13804,6 +13859,7 @@
       <c r="M292" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N292" s="0"/>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="30" t="n">
@@ -13841,6 +13897,7 @@
       <c r="M293" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N293" s="0"/>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="30" t="n">
@@ -13878,6 +13935,7 @@
       <c r="M294" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N294" s="0"/>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="30" t="n">
@@ -13915,6 +13973,7 @@
       <c r="M295" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N295" s="0"/>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="17" t="n">
@@ -13952,6 +14011,7 @@
       <c r="M296" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N296" s="0"/>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="17" t="n">
@@ -13991,6 +14051,7 @@
       <c r="M297" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N297" s="0"/>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="17" t="n">
@@ -14026,6 +14087,7 @@
       <c r="M298" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N298" s="0"/>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="17" t="n">
@@ -14061,6 +14123,7 @@
       <c r="M299" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N299" s="0"/>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="17" t="n">
@@ -14096,6 +14159,7 @@
       <c r="M300" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N300" s="0"/>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="17" t="n">
@@ -14131,6 +14195,7 @@
       <c r="M301" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N301" s="0"/>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="17" t="n">
@@ -14166,6 +14231,7 @@
       <c r="M302" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N302" s="0"/>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="17" t="n">
@@ -14201,6 +14267,7 @@
       <c r="M303" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N303" s="0"/>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="17" t="n">
@@ -14236,6 +14303,7 @@
       <c r="M304" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N304" s="0"/>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="17" t="n">
@@ -14273,6 +14341,7 @@
       <c r="M305" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N305" s="0"/>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="17" t="n">
@@ -14310,6 +14379,7 @@
       <c r="M306" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N306" s="0"/>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="17" t="n">
@@ -14347,6 +14417,7 @@
       <c r="M307" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N307" s="0"/>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="17" t="n">
@@ -14384,6 +14455,7 @@
       <c r="M308" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N308" s="0"/>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="30" t="n">
@@ -14421,6 +14493,7 @@
       <c r="M309" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N309" s="0"/>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="30" t="n">
@@ -14458,6 +14531,7 @@
       <c r="M310" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N310" s="0"/>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="30" t="n">
@@ -14495,6 +14569,7 @@
       <c r="M311" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N311" s="0"/>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="17" t="n">
@@ -14530,6 +14605,7 @@
       <c r="M312" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N312" s="0"/>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="17" t="n">
@@ -14565,6 +14641,7 @@
       <c r="M313" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N313" s="0"/>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="17" t="n">
@@ -14602,6 +14679,7 @@
       <c r="M314" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N314" s="0"/>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="17" t="n">
@@ -14639,6 +14717,7 @@
       <c r="M315" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N315" s="0"/>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="17" t="n">
@@ -14674,6 +14753,7 @@
       <c r="M316" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N316" s="0"/>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="17" t="n">
@@ -14709,6 +14789,7 @@
       <c r="M317" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N317" s="0"/>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="17" t="n">
@@ -14748,6 +14829,7 @@
       <c r="M318" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N318" s="0"/>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="17" t="n">
@@ -14785,6 +14867,7 @@
       <c r="M319" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N319" s="0"/>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="17" t="n">
@@ -14822,6 +14905,7 @@
       <c r="M320" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N320" s="0"/>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="17" t="n">
@@ -14859,6 +14943,7 @@
       <c r="M321" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N321" s="0"/>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="30" t="n">
@@ -14896,6 +14981,7 @@
       <c r="M322" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N322" s="0"/>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="30" t="n">
@@ -14933,6 +15019,7 @@
       <c r="M323" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N323" s="0"/>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="30" t="n">
@@ -14970,6 +15057,7 @@
       <c r="M324" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N324" s="0"/>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="30" t="n">
@@ -15007,6 +15095,7 @@
       <c r="M325" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N325" s="0"/>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="17" t="n">
@@ -15044,6 +15133,7 @@
       <c r="M326" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N326" s="0"/>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="30" t="n">
@@ -15081,6 +15171,7 @@
       <c r="M327" s="34" t="s">
         <v>19</v>
       </c>
+      <c r="N327" s="0"/>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="30" t="n">
@@ -15118,6 +15209,7 @@
       <c r="M328" s="34" t="s">
         <v>19</v>
       </c>
+      <c r="N328" s="0"/>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="17" t="n">
@@ -15155,6 +15247,7 @@
       <c r="M329" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N329" s="0"/>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="30" t="n">
@@ -15194,6 +15287,7 @@
       <c r="M330" s="34" t="s">
         <v>42</v>
       </c>
+      <c r="N330" s="0"/>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="17" t="n">
@@ -15231,6 +15325,7 @@
       <c r="M331" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N331" s="0"/>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="17" t="n">
@@ -15268,6 +15363,7 @@
       <c r="M332" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N332" s="0"/>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="17" t="n">
@@ -15305,6 +15401,7 @@
       <c r="M333" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N333" s="0"/>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="17" t="n">
@@ -15342,6 +15439,7 @@
       <c r="M334" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="N334" s="0"/>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="30" t="n">
@@ -15379,6 +15477,7 @@
       <c r="M335" s="34" t="s">
         <v>19</v>
       </c>
+      <c r="N335" s="0"/>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="30" t="n">
@@ -15416,6 +15515,7 @@
       <c r="M336" s="34" t="s">
         <v>19</v>
       </c>
+      <c r="N336" s="0"/>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="30" t="n">
@@ -15453,6 +15553,7 @@
       <c r="M337" s="34" t="s">
         <v>19</v>
       </c>
+      <c r="N337" s="0"/>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="17" t="n">
@@ -15490,6 +15591,7 @@
       <c r="M338" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N338" s="0"/>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="17" t="n">
@@ -15527,6 +15629,7 @@
       <c r="M339" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="N339" s="0"/>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="30" t="n">
@@ -34213,252 +34316,252 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F4">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>T4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>U9="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>U10="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>U7="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>U8="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C530:F530">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>O532="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B400:F400">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N394="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B401:F401">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N395="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B389:F389">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>U385="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>U11="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B532:F532">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N534="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B531:F531">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N533="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B545:F545">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>J545="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B390:F390">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>U386="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B391:F391">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>U387="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B396:F396">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N391="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B543:F543">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>J543="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B385:F386">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>U381="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>T7="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>T10="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:D8">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>T8="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:D11">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>T11="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B404">
     <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N398="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B405">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>N399="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
     <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
     <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
     <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
     <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
     <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
     <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
     <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
     <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
     <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
     <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
     <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
     <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
     <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
     <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
     <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
     <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
     <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
     <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>W4="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">

</xml_diff>